<commit_message>
É possível remover as informações a partir do código de uma partida; lógica de salvamento alterada
</commit_message>
<xml_diff>
--- a/Excel/Sumula_Teste_T01B01.xlsx
+++ b/Excel/Sumula_Teste_T01B01.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A371D79A-C127-436E-831B-41857224199D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Roberto\Documents\Programacao\projetos-pessoais\associacao-futebol\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20943197-0C99-4485-9074-8D0F701B14DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="1" r:id="rId1"/>
@@ -17,17 +22,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -153,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,21 +176,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="23">
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -212,46 +278,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04FC458E-162D-4E2E-AF69-689F334082C8}" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04FC458E-162D-4E2E-AF69-689F334082C8}" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="22" dataDxfId="16">
   <autoFilter ref="A1:E16" xr:uid="{04FC458E-162D-4E2E-AF69-689F334082C8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{01182F49-E3B6-4318-B325-16E600D16565}" name="Baba"/>
-    <tableColumn id="2" xr3:uid="{FEF1A800-37FF-45E3-A48A-26008128B6A5}" name="Jogador"/>
-    <tableColumn id="3" xr3:uid="{2252E8E2-E700-4783-B765-98CCCED37330}" name="Time"/>
-    <tableColumn id="5" xr3:uid="{3805501C-D487-41C8-AF9B-CE0267FED812}" name="Gols"/>
-    <tableColumn id="6" xr3:uid="{585EACE7-E288-48A8-B347-1FDEE2212FA4}" name="Assistências"/>
+    <tableColumn id="1" xr3:uid="{01182F49-E3B6-4318-B325-16E600D16565}" name="Baba" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{FEF1A800-37FF-45E3-A48A-26008128B6A5}" name="Jogador" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2252E8E2-E700-4783-B765-98CCCED37330}" name="Time" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{3805501C-D487-41C8-AF9B-CE0267FED812}" name="Gols" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{585EACE7-E288-48A8-B347-1FDEE2212FA4}" name="Assistências" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0D62CAB6-5F84-4A18-8C77-97430EDB3045}" name="Table13" displayName="Table13" ref="A1:F4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0D62CAB6-5F84-4A18-8C77-97430EDB3045}" name="Table13" displayName="Table13" ref="A1:F4" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:F4" xr:uid="{04FC458E-162D-4E2E-AF69-689F334082C8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{700BC8C2-3F3A-49CD-B702-F27A34D0AD70}" name="Baba"/>
-    <tableColumn id="3" xr3:uid="{F9950AAE-3CB5-4F50-854F-6124CD59B5A9}" name="Time"/>
-    <tableColumn id="4" xr3:uid="{9C4BC1BC-B3D9-4750-9263-535201EBDB59}" name="Campeão"/>
-    <tableColumn id="9" xr3:uid="{35CD1899-FA04-4AD8-9B57-C4FC7E8E37BA}" name="Vitórias"/>
-    <tableColumn id="8" xr3:uid="{DAB12672-F2BC-4EAD-AB01-8D8CF3D907BF}" name="Empates"/>
-    <tableColumn id="7" xr3:uid="{6BD16F69-2FAB-4D92-A3CA-2E3D24B339A6}" name="Derrotas"/>
+    <tableColumn id="1" xr3:uid="{700BC8C2-3F3A-49CD-B702-F27A34D0AD70}" name="Baba" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{F9950AAE-3CB5-4F50-854F-6124CD59B5A9}" name="Time" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{9C4BC1BC-B3D9-4750-9263-535201EBDB59}" name="Campeão" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{35CD1899-FA04-4AD8-9B57-C4FC7E8E37BA}" name="Vitórias" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{DAB12672-F2BC-4EAD-AB01-8D8CF3D907BF}" name="Empates" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{6BD16F69-2FAB-4D92-A3CA-2E3D24B339A6}" name="Derrotas" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE2F048A-12C1-47B3-8490-CCCB25722A76}" name="Table14" displayName="Table14" ref="A1:H2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE2F048A-12C1-47B3-8490-CCCB25722A76}" name="Table14" displayName="Table14" ref="A1:H2" totalsRowShown="0" dataDxfId="0">
   <autoFilter ref="A1:H2" xr:uid="{04FC458E-162D-4E2E-AF69-689F334082C8}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E3775AF1-7F45-4DCE-86BC-3D85B0A7413B}" name="Baba"/>
-    <tableColumn id="4" xr3:uid="{0C56AD3D-A7B0-4BD5-8264-31B3341790B3}" name="Data"/>
-    <tableColumn id="5" xr3:uid="{08060C07-5883-4731-9097-7F21E4A9FAB5}" name="Início"/>
-    <tableColumn id="6" xr3:uid="{0C3232FE-38C4-4005-A4EB-33CADBFAD8C9}" name="Fim"/>
-    <tableColumn id="9" xr3:uid="{95DB3544-C87B-4EDE-9E7B-AEC1D111E334}" name="Árbitro" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{3EB0C095-1FC4-4A10-B852-CAB61CB5FD55}" name="Nota" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{BB5C5ABF-C527-470D-B85F-EB613D693DF2}" name="Campo"/>
-    <tableColumn id="11" xr3:uid="{6E3DA2F7-3DA3-4A6E-8348-F9F4D3A0EFA1}" name="Coordenadas"/>
+    <tableColumn id="1" xr3:uid="{E3775AF1-7F45-4DCE-86BC-3D85B0A7413B}" name="Baba" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{0C56AD3D-A7B0-4BD5-8264-31B3341790B3}" name="Data" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{08060C07-5883-4731-9097-7F21E4A9FAB5}" name="Início" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{0C3232FE-38C4-4005-A4EB-33CADBFAD8C9}" name="Fim" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{95DB3544-C87B-4EDE-9E7B-AEC1D111E334}" name="Árbitro" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{3EB0C095-1FC4-4A10-B852-CAB61CB5FD55}" name="Nota" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{BB5C5ABF-C527-470D-B85F-EB613D693DF2}" name="Campo" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{6E3DA2F7-3DA3-4A6E-8348-F9F4D3A0EFA1}" name="Coordenadas" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -576,291 +642,292 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -873,19 +940,22 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,67 +975,68 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -978,22 +1049,24 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1019,33 +1092,34 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
         <v>45521</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>